<commit_message>
decision tress and random forests
</commit_message>
<xml_diff>
--- a/MLTracker.xlsx
+++ b/MLTracker.xlsx
@@ -1,37 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caitlin\Desktop\cwrubootcamp\Homework\DonorsChoose\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Code\DonorsChoose\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0366E4C7-6E4C-4FA1-883C-5CCECC4A364F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{EAB151D4-567B-431C-93A2-CBA4BFD5AB76}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6900" yWindow="4632" windowWidth="23040" windowHeight="11028" xr2:uid="{8BE3917C-5764-4427-A3FC-3DBEDE359AE0}"/>
+    <workbookView xWindow="6900" yWindow="4635" windowWidth="23040" windowHeight="11025" xr2:uid="{8BE3917C-5764-4427-A3FC-3DBEDE359AE0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Logistic Regression" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="45">
   <si>
     <t>school_metro</t>
   </si>
@@ -111,20 +105,68 @@
     <t>eligible_almost_home_match</t>
   </si>
   <si>
-    <t>date_posted</t>
-  </si>
-  <si>
     <t>r2</t>
   </si>
   <si>
     <t>mse</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>dataset</t>
+  </si>
+  <si>
+    <t>no-metro-no-sales</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>logistic regression</t>
+  </si>
+  <si>
+    <t>decision tree</t>
+  </si>
+  <si>
+    <t>random forest</t>
+  </si>
+  <si>
+    <t>K Nearest Neighbors</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>fixed characteristics</t>
+  </si>
+  <si>
+    <t>subjects</t>
+  </si>
+  <si>
+    <t>subjects w/ money</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>students + money</t>
+  </si>
+  <si>
+    <t>all simplified</t>
+  </si>
+  <si>
+    <t>simplified money</t>
+  </si>
+  <si>
+    <t>fixed + match</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,16 +174,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -149,15 +215,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="2" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -469,104 +557,1249 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3B90DFA-DE1E-475C-9FD6-036A41419806}">
-  <dimension ref="A1:AC1"/>
+  <dimension ref="A1:AE33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10:AE13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="24" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="26" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="27.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>15</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" t="s">
         <v>16</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" t="s">
         <v>17</v>
       </c>
-      <c r="U1" t="s">
+      <c r="X1" t="s">
         <v>18</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Y1" t="s">
         <v>19</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Z1" t="s">
         <v>20</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AA1" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AB1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AC1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AD1" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AE1" t="s">
         <v>25</v>
       </c>
-      <c r="AC1" t="s">
-        <v>26</v>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2">
+        <v>-0.39839999999999998</v>
+      </c>
+      <c r="C2">
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>28</v>
+      </c>
+      <c r="R2" t="s">
+        <v>28</v>
+      </c>
+      <c r="S2" t="s">
+        <v>28</v>
+      </c>
+      <c r="T2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>-0.7782</v>
+      </c>
+      <c r="C3">
+        <v>0.37380000000000002</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O3" t="s">
+        <v>28</v>
+      </c>
+      <c r="P3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>28</v>
+      </c>
+      <c r="R3" t="s">
+        <v>28</v>
+      </c>
+      <c r="S3" t="s">
+        <v>28</v>
+      </c>
+      <c r="T3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB3"/>
+      <c r="AC3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O4" t="s">
+        <v>28</v>
+      </c>
+      <c r="P4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O5" t="s">
+        <v>28</v>
+      </c>
+      <c r="P5" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>28</v>
+      </c>
+      <c r="R5" t="s">
+        <v>28</v>
+      </c>
+      <c r="S5" t="s">
+        <v>28</v>
+      </c>
+      <c r="T5" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6">
+        <v>-0.40029999999999999</v>
+      </c>
+      <c r="C6">
+        <v>0.2944</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" t="s">
+        <v>28</v>
+      </c>
+      <c r="P6" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>28</v>
+      </c>
+      <c r="R6" t="s">
+        <v>28</v>
+      </c>
+      <c r="S6" t="s">
+        <v>28</v>
+      </c>
+      <c r="T6" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>-0.78469999999999995</v>
+      </c>
+      <c r="C7">
+        <v>0.37519999999999998</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" t="s">
+        <v>28</v>
+      </c>
+      <c r="P7" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>28</v>
+      </c>
+      <c r="R7" t="s">
+        <v>28</v>
+      </c>
+      <c r="S7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T7" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P8" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>28</v>
+      </c>
+      <c r="R8" t="s">
+        <v>28</v>
+      </c>
+      <c r="S8" t="s">
+        <v>28</v>
+      </c>
+      <c r="T8" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" t="s">
+        <v>28</v>
+      </c>
+      <c r="P9" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>28</v>
+      </c>
+      <c r="R9" t="s">
+        <v>28</v>
+      </c>
+      <c r="S9" t="s">
+        <v>28</v>
+      </c>
+      <c r="T9" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10">
+        <v>-0.4299</v>
+      </c>
+      <c r="C10">
+        <v>0.30059999999999998</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" t="s">
+        <v>28</v>
+      </c>
+      <c r="J10" t="s">
+        <v>28</v>
+      </c>
+      <c r="K10" t="s">
+        <v>28</v>
+      </c>
+      <c r="L10" t="s">
+        <v>28</v>
+      </c>
+      <c r="M10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N10" t="s">
+        <v>28</v>
+      </c>
+      <c r="O10" t="s">
+        <v>28</v>
+      </c>
+      <c r="S10" t="s">
+        <v>28</v>
+      </c>
+      <c r="T10" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB10"/>
+      <c r="AC10"/>
+    </row>
+    <row r="11" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>-0.4299</v>
+      </c>
+      <c r="C11">
+        <v>0.30059999999999998</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M11" t="s">
+        <v>28</v>
+      </c>
+      <c r="N11" t="s">
+        <v>28</v>
+      </c>
+      <c r="O11" t="s">
+        <v>28</v>
+      </c>
+      <c r="S11" t="s">
+        <v>28</v>
+      </c>
+      <c r="T11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12" t="s">
+        <v>28</v>
+      </c>
+      <c r="J12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M12" t="s">
+        <v>28</v>
+      </c>
+      <c r="N12" t="s">
+        <v>28</v>
+      </c>
+      <c r="O12" t="s">
+        <v>28</v>
+      </c>
+      <c r="S12" t="s">
+        <v>28</v>
+      </c>
+      <c r="T12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB12"/>
+      <c r="AC12"/>
+    </row>
+    <row r="13" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" t="s">
+        <v>28</v>
+      </c>
+      <c r="J13" t="s">
+        <v>28</v>
+      </c>
+      <c r="K13" t="s">
+        <v>28</v>
+      </c>
+      <c r="L13" t="s">
+        <v>28</v>
+      </c>
+      <c r="M13" t="s">
+        <v>28</v>
+      </c>
+      <c r="N13" t="s">
+        <v>28</v>
+      </c>
+      <c r="O13" t="s">
+        <v>28</v>
+      </c>
+      <c r="S13" t="s">
+        <v>28</v>
+      </c>
+      <c r="T13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14">
+        <v>-0.4299</v>
+      </c>
+      <c r="C14">
+        <v>0.20066000000000001</v>
+      </c>
+      <c r="D14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" t="s">
+        <v>28</v>
+      </c>
+      <c r="J14" t="s">
+        <v>28</v>
+      </c>
+      <c r="K14" t="s">
+        <v>28</v>
+      </c>
+      <c r="L14" t="s">
+        <v>28</v>
+      </c>
+      <c r="M14" t="s">
+        <v>28</v>
+      </c>
+      <c r="N14" t="s">
+        <v>28</v>
+      </c>
+      <c r="O14" t="s">
+        <v>28</v>
+      </c>
+      <c r="S14" t="s">
+        <v>28</v>
+      </c>
+      <c r="T14" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB14"/>
+      <c r="AC14"/>
+      <c r="AD14" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>-0.43049999999999999</v>
+      </c>
+      <c r="C15">
+        <v>0.30070000000000002</v>
+      </c>
+      <c r="D15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" t="s">
+        <v>28</v>
+      </c>
+      <c r="H15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I15" t="s">
+        <v>28</v>
+      </c>
+      <c r="J15" t="s">
+        <v>28</v>
+      </c>
+      <c r="K15" t="s">
+        <v>28</v>
+      </c>
+      <c r="L15" t="s">
+        <v>28</v>
+      </c>
+      <c r="M15" t="s">
+        <v>28</v>
+      </c>
+      <c r="N15" t="s">
+        <v>28</v>
+      </c>
+      <c r="O15" t="s">
+        <v>28</v>
+      </c>
+      <c r="S15" t="s">
+        <v>28</v>
+      </c>
+      <c r="T15" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" t="s">
+        <v>28</v>
+      </c>
+      <c r="H17" t="s">
+        <v>28</v>
+      </c>
+      <c r="I17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J17" t="s">
+        <v>28</v>
+      </c>
+      <c r="K17" t="s">
+        <v>28</v>
+      </c>
+      <c r="L17" t="s">
+        <v>28</v>
+      </c>
+      <c r="M17" t="s">
+        <v>28</v>
+      </c>
+      <c r="N17" t="s">
+        <v>28</v>
+      </c>
+      <c r="O17" t="s">
+        <v>28</v>
+      </c>
+      <c r="S17" t="s">
+        <v>28</v>
+      </c>
+      <c r="T17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18">
+        <v>-0.40200000000000002</v>
+      </c>
+      <c r="C18">
+        <v>-0.29480000000000001</v>
+      </c>
+      <c r="D18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>-0.62329999999999997</v>
+      </c>
+      <c r="C19">
+        <v>0.34129999999999999</v>
+      </c>
+      <c r="D19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD20" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22">
+        <v>-0.4299</v>
+      </c>
+      <c r="C22">
+        <v>0.30059999999999998</v>
+      </c>
+      <c r="D22" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" t="s">
+        <v>30</v>
+      </c>
+      <c r="P22" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>28</v>
+      </c>
+      <c r="R22" t="s">
+        <v>28</v>
+      </c>
+      <c r="T22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>-0.43070000000000003</v>
+      </c>
+      <c r="C23">
+        <v>0.30080000000000001</v>
+      </c>
+      <c r="D23" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" t="s">
+        <v>30</v>
+      </c>
+      <c r="P23" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>28</v>
+      </c>
+      <c r="R23" t="s">
+        <v>28</v>
+      </c>
+      <c r="T23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>30</v>
+      </c>
+      <c r="P24" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>28</v>
+      </c>
+      <c r="R24" t="s">
+        <v>28</v>
+      </c>
+      <c r="T24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>30</v>
+      </c>
+      <c r="P25" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>28</v>
+      </c>
+      <c r="R25" t="s">
+        <v>28</v>
+      </c>
+      <c r="T25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26">
+        <v>-0.40920000000000001</v>
+      </c>
+      <c r="C26">
+        <v>0.29630000000000001</v>
+      </c>
+      <c r="D26" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" t="s">
+        <v>30</v>
+      </c>
+      <c r="P26" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>28</v>
+      </c>
+      <c r="R26" t="s">
+        <v>28</v>
+      </c>
+      <c r="T26" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>-0.81430000000000002</v>
+      </c>
+      <c r="C27">
+        <v>0.38150000000000001</v>
+      </c>
+      <c r="D27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30">
+        <v>-0.40260000000000001</v>
+      </c>
+      <c r="C30">
+        <v>0.2949</v>
+      </c>
+      <c r="D30" t="s">
+        <v>32</v>
+      </c>
+      <c r="E30" t="s">
+        <v>30</v>
+      </c>
+      <c r="S30" t="s">
+        <v>28</v>
+      </c>
+      <c r="T30" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="1">
+        <v>-0.83799999999999997</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0.38640000000000002</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="S31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB31" s="3"/>
+      <c r="AC31" s="3"/>
+    </row>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more models and file reorganization
</commit_message>
<xml_diff>
--- a/MLTracker.xlsx
+++ b/MLTracker.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Code\DonorsChoose\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1B133DDD-D1B1-4054-A6CA-E792E8454058}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BA419E11-9BC6-4DF5-836A-BCA52F81E355}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6900" yWindow="4635" windowWidth="23040" windowHeight="11025" xr2:uid="{8BE3917C-5764-4427-A3FC-3DBEDE359AE0}"/>
+    <workbookView xWindow="6900" yWindow="4635" windowWidth="23040" windowHeight="11025" activeTab="1" xr2:uid="{8BE3917C-5764-4427-A3FC-3DBEDE359AE0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Logistic Regression" sheetId="1" r:id="rId1"/>
+    <sheet name="No Metro" sheetId="1" r:id="rId1"/>
+    <sheet name="Metro" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="46">
   <si>
     <t>school_metro</t>
   </si>
@@ -160,6 +161,9 @@
   </si>
   <si>
     <t>fixed + match</t>
+  </si>
+  <si>
+    <t>metro_included</t>
   </si>
 </sst>
 </file>
@@ -236,11 +240,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -559,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3B90DFA-DE1E-475C-9FD6-036A41419806}">
   <dimension ref="A1:AE33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:XFD33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -912,6 +917,12 @@
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>-0.44740000000000002</v>
+      </c>
+      <c r="C5">
+        <v>0.30430000000000001</v>
+      </c>
       <c r="D5" t="s">
         <v>35</v>
       </c>
@@ -1083,6 +1094,9 @@
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
       <c r="E8" t="s">
         <v>30</v>
       </c>
@@ -1124,6 +1138,15 @@
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>-0.51149999999999995</v>
+      </c>
+      <c r="C9">
+        <v>0.31780000000000003</v>
+      </c>
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
       <c r="E9" t="s">
         <v>30</v>
       </c>
@@ -1264,6 +1287,9 @@
       </c>
     </row>
     <row r="12" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
       <c r="E12" t="s">
         <v>30</v>
       </c>
@@ -1304,6 +1330,9 @@
       <c r="AC12"/>
     </row>
     <row r="13" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>35</v>
+      </c>
       <c r="E13" t="s">
         <v>30</v>
       </c>
@@ -1453,11 +1482,17 @@
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>34</v>
+      </c>
       <c r="E16" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>35</v>
+      </c>
       <c r="E17" t="s">
         <v>30</v>
       </c>
@@ -1551,6 +1586,9 @@
       </c>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>34</v>
+      </c>
       <c r="E20" t="s">
         <v>30</v>
       </c>
@@ -1568,6 +1606,9 @@
       </c>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>35</v>
+      </c>
       <c r="E21" t="s">
         <v>30</v>
       </c>
@@ -1640,6 +1681,9 @@
       </c>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>34</v>
+      </c>
       <c r="E24" t="s">
         <v>30</v>
       </c>
@@ -1657,6 +1701,9 @@
       </c>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>35</v>
+      </c>
       <c r="E25" t="s">
         <v>30</v>
       </c>
@@ -1721,15 +1768,75 @@
       <c r="E27" t="s">
         <v>30</v>
       </c>
+      <c r="P27" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>28</v>
+      </c>
+      <c r="R27" t="s">
+        <v>28</v>
+      </c>
+      <c r="T27" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>34</v>
+      </c>
       <c r="E28" t="s">
         <v>30</v>
       </c>
+      <c r="P28" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>28</v>
+      </c>
+      <c r="R28" t="s">
+        <v>28</v>
+      </c>
+      <c r="T28" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>35</v>
+      </c>
       <c r="E29" t="s">
         <v>30</v>
+      </c>
+      <c r="P29" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>28</v>
+      </c>
+      <c r="R29" t="s">
+        <v>28</v>
+      </c>
+      <c r="T29" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.25">
@@ -1771,7 +1878,7 @@
       <c r="C31" s="1">
         <v>0.38640000000000002</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" t="s">
         <v>33</v>
       </c>
       <c r="E31" s="1" t="s">
@@ -1802,14 +1909,1445 @@
       <c r="C32">
         <v>0.34160000000000001</v>
       </c>
+      <c r="D32" t="s">
+        <v>34</v>
+      </c>
       <c r="E32" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="S32" t="s">
+        <v>28</v>
+      </c>
+      <c r="T32" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="4:31" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>35</v>
+      </c>
       <c r="E33" t="s">
         <v>30</v>
       </c>
+      <c r="S33" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T33" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="U33" s="1"/>
+      <c r="V33" s="1"/>
+      <c r="W33" s="1"/>
+      <c r="X33" s="1"/>
+      <c r="Y33" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z33" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA33" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB33" s="3"/>
+      <c r="AC33" s="3"/>
+      <c r="AD33" s="1"/>
+      <c r="AE33" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FD12F4D-DDDC-4B63-8E0E-DCA71E86A3ED}">
+  <dimension ref="A1:AE33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.5703125" customWidth="1"/>
+    <col min="17" max="17" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="24" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="27.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="26" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="27.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R1" t="s">
+        <v>12</v>
+      </c>
+      <c r="S1" t="s">
+        <v>13</v>
+      </c>
+      <c r="T1" t="s">
+        <v>14</v>
+      </c>
+      <c r="U1" t="s">
+        <v>15</v>
+      </c>
+      <c r="V1" t="s">
+        <v>16</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2">
+        <v>-0.38840000000000002</v>
+      </c>
+      <c r="C2">
+        <v>0.28870000000000001</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>28</v>
+      </c>
+      <c r="R2" t="s">
+        <v>28</v>
+      </c>
+      <c r="S2" t="s">
+        <v>28</v>
+      </c>
+      <c r="T2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O3" t="s">
+        <v>28</v>
+      </c>
+      <c r="P3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>28</v>
+      </c>
+      <c r="R3" t="s">
+        <v>28</v>
+      </c>
+      <c r="S3" t="s">
+        <v>28</v>
+      </c>
+      <c r="T3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O4" t="s">
+        <v>28</v>
+      </c>
+      <c r="P4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O5" t="s">
+        <v>28</v>
+      </c>
+      <c r="P5" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>28</v>
+      </c>
+      <c r="R5" t="s">
+        <v>28</v>
+      </c>
+      <c r="S5" t="s">
+        <v>28</v>
+      </c>
+      <c r="T5" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6">
+        <v>-0.4118</v>
+      </c>
+      <c r="C6">
+        <v>0.29349999999999998</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" t="s">
+        <v>28</v>
+      </c>
+      <c r="P6" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>28</v>
+      </c>
+      <c r="R6" t="s">
+        <v>28</v>
+      </c>
+      <c r="S6" t="s">
+        <v>28</v>
+      </c>
+      <c r="T6" t="s">
+        <v>28</v>
+      </c>
+      <c r="W6"/>
+      <c r="X6"/>
+      <c r="Y6" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB6" s="2"/>
+      <c r="AC6" s="2"/>
+      <c r="AD6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" t="s">
+        <v>28</v>
+      </c>
+      <c r="P7" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>28</v>
+      </c>
+      <c r="R7" t="s">
+        <v>28</v>
+      </c>
+      <c r="S7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T7" t="s">
+        <v>28</v>
+      </c>
+      <c r="W7"/>
+      <c r="X7"/>
+      <c r="Y7" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB7" s="2"/>
+      <c r="AC7" s="2"/>
+      <c r="AD7" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P8" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>28</v>
+      </c>
+      <c r="R8" t="s">
+        <v>28</v>
+      </c>
+      <c r="S8" t="s">
+        <v>28</v>
+      </c>
+      <c r="T8" t="s">
+        <v>28</v>
+      </c>
+      <c r="W8"/>
+      <c r="X8"/>
+      <c r="Y8" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="2"/>
+      <c r="AD8" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" t="s">
+        <v>28</v>
+      </c>
+      <c r="P9" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>28</v>
+      </c>
+      <c r="R9" t="s">
+        <v>28</v>
+      </c>
+      <c r="S9" t="s">
+        <v>28</v>
+      </c>
+      <c r="T9" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10">
+        <v>-0.41830000000000001</v>
+      </c>
+      <c r="C10">
+        <v>0.2949</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" t="s">
+        <v>28</v>
+      </c>
+      <c r="J10" t="s">
+        <v>28</v>
+      </c>
+      <c r="K10" t="s">
+        <v>28</v>
+      </c>
+      <c r="L10" t="s">
+        <v>28</v>
+      </c>
+      <c r="M10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N10" t="s">
+        <v>28</v>
+      </c>
+      <c r="O10" t="s">
+        <v>28</v>
+      </c>
+      <c r="S10" t="s">
+        <v>28</v>
+      </c>
+      <c r="T10" t="s">
+        <v>28</v>
+      </c>
+      <c r="W10"/>
+      <c r="X10"/>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M11" t="s">
+        <v>28</v>
+      </c>
+      <c r="N11" t="s">
+        <v>28</v>
+      </c>
+      <c r="O11" t="s">
+        <v>28</v>
+      </c>
+      <c r="S11" t="s">
+        <v>28</v>
+      </c>
+      <c r="T11" t="s">
+        <v>28</v>
+      </c>
+      <c r="W11"/>
+      <c r="X11"/>
+      <c r="AB11" s="2"/>
+      <c r="AC11" s="2"/>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12" t="s">
+        <v>28</v>
+      </c>
+      <c r="J12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M12" t="s">
+        <v>28</v>
+      </c>
+      <c r="N12" t="s">
+        <v>28</v>
+      </c>
+      <c r="O12" t="s">
+        <v>28</v>
+      </c>
+      <c r="S12" t="s">
+        <v>28</v>
+      </c>
+      <c r="T12" t="s">
+        <v>28</v>
+      </c>
+      <c r="W12"/>
+      <c r="X12"/>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" t="s">
+        <v>28</v>
+      </c>
+      <c r="J13" t="s">
+        <v>28</v>
+      </c>
+      <c r="K13" t="s">
+        <v>28</v>
+      </c>
+      <c r="L13" t="s">
+        <v>28</v>
+      </c>
+      <c r="M13" t="s">
+        <v>28</v>
+      </c>
+      <c r="N13" t="s">
+        <v>28</v>
+      </c>
+      <c r="O13" t="s">
+        <v>28</v>
+      </c>
+      <c r="S13" t="s">
+        <v>28</v>
+      </c>
+      <c r="T13" t="s">
+        <v>28</v>
+      </c>
+      <c r="W13"/>
+      <c r="X13"/>
+      <c r="AB13" s="2"/>
+      <c r="AC13" s="2"/>
+    </row>
+    <row r="14" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14">
+        <v>-0.41830000000000001</v>
+      </c>
+      <c r="C14">
+        <v>0.2949</v>
+      </c>
+      <c r="D14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" t="s">
+        <v>28</v>
+      </c>
+      <c r="J14" t="s">
+        <v>28</v>
+      </c>
+      <c r="K14" t="s">
+        <v>28</v>
+      </c>
+      <c r="L14" t="s">
+        <v>28</v>
+      </c>
+      <c r="M14" t="s">
+        <v>28</v>
+      </c>
+      <c r="N14" t="s">
+        <v>28</v>
+      </c>
+      <c r="O14" t="s">
+        <v>28</v>
+      </c>
+      <c r="S14" t="s">
+        <v>28</v>
+      </c>
+      <c r="T14" t="s">
+        <v>28</v>
+      </c>
+      <c r="W14"/>
+      <c r="X14"/>
+      <c r="AD14" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" t="s">
+        <v>28</v>
+      </c>
+      <c r="H15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I15" t="s">
+        <v>28</v>
+      </c>
+      <c r="J15" t="s">
+        <v>28</v>
+      </c>
+      <c r="K15" t="s">
+        <v>28</v>
+      </c>
+      <c r="L15" t="s">
+        <v>28</v>
+      </c>
+      <c r="M15" t="s">
+        <v>28</v>
+      </c>
+      <c r="N15" t="s">
+        <v>28</v>
+      </c>
+      <c r="O15" t="s">
+        <v>28</v>
+      </c>
+      <c r="S15" t="s">
+        <v>28</v>
+      </c>
+      <c r="T15" t="s">
+        <v>28</v>
+      </c>
+      <c r="W15"/>
+      <c r="X15"/>
+      <c r="AB15" s="2"/>
+      <c r="AC15" s="2"/>
+      <c r="AD15" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" t="s">
+        <v>28</v>
+      </c>
+      <c r="W16"/>
+      <c r="X16"/>
+      <c r="AB16" s="2"/>
+      <c r="AC16" s="2"/>
+      <c r="AD16" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" t="s">
+        <v>28</v>
+      </c>
+      <c r="H17" t="s">
+        <v>28</v>
+      </c>
+      <c r="I17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J17" t="s">
+        <v>28</v>
+      </c>
+      <c r="K17" t="s">
+        <v>28</v>
+      </c>
+      <c r="L17" t="s">
+        <v>28</v>
+      </c>
+      <c r="M17" t="s">
+        <v>28</v>
+      </c>
+      <c r="N17" t="s">
+        <v>28</v>
+      </c>
+      <c r="O17" t="s">
+        <v>28</v>
+      </c>
+      <c r="S17" t="s">
+        <v>28</v>
+      </c>
+      <c r="T17" t="s">
+        <v>28</v>
+      </c>
+      <c r="W17"/>
+      <c r="X17"/>
+      <c r="AB17" s="2"/>
+      <c r="AC17" s="2"/>
+      <c r="AD17" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18">
+        <v>-0.39600000000000002</v>
+      </c>
+      <c r="C18">
+        <v>0.2903</v>
+      </c>
+      <c r="D18" t="s">
+        <v>32</v>
+      </c>
+      <c r="W18"/>
+      <c r="X18"/>
+      <c r="Y18" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB18" s="2"/>
+      <c r="AC18" s="2"/>
+      <c r="AD18" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>33</v>
+      </c>
+      <c r="W19"/>
+      <c r="X19"/>
+      <c r="Y19" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB19" s="2"/>
+      <c r="AC19" s="2"/>
+      <c r="AD19" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>34</v>
+      </c>
+      <c r="W20"/>
+      <c r="X20"/>
+      <c r="Y20" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB20" s="2"/>
+      <c r="AC20" s="2"/>
+      <c r="AD20" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>35</v>
+      </c>
+      <c r="W21"/>
+      <c r="X21"/>
+      <c r="Y21" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB21" s="2"/>
+      <c r="AC21" s="2"/>
+      <c r="AD21" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22">
+        <v>-0.41830000000000001</v>
+      </c>
+      <c r="C22">
+        <v>0.2949</v>
+      </c>
+      <c r="D22" t="s">
+        <v>32</v>
+      </c>
+      <c r="P22" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>28</v>
+      </c>
+      <c r="R22" t="s">
+        <v>28</v>
+      </c>
+      <c r="T22" t="s">
+        <v>28</v>
+      </c>
+      <c r="W22"/>
+      <c r="X22"/>
+      <c r="AB22" s="2"/>
+      <c r="AC22" s="2"/>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>33</v>
+      </c>
+      <c r="P23" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>28</v>
+      </c>
+      <c r="R23" t="s">
+        <v>28</v>
+      </c>
+      <c r="T23" t="s">
+        <v>28</v>
+      </c>
+      <c r="W23"/>
+      <c r="X23"/>
+      <c r="AB23" s="2"/>
+      <c r="AC23" s="2"/>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>34</v>
+      </c>
+      <c r="P24" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>28</v>
+      </c>
+      <c r="R24" t="s">
+        <v>28</v>
+      </c>
+      <c r="T24" t="s">
+        <v>28</v>
+      </c>
+      <c r="W24"/>
+      <c r="X24"/>
+      <c r="AB24" s="2"/>
+      <c r="AC24" s="2"/>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>35</v>
+      </c>
+      <c r="P25" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>28</v>
+      </c>
+      <c r="R25" t="s">
+        <v>28</v>
+      </c>
+      <c r="T25" t="s">
+        <v>28</v>
+      </c>
+      <c r="W25"/>
+      <c r="X25"/>
+      <c r="AB25" s="2"/>
+      <c r="AC25" s="2"/>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26">
+        <v>-0.39739999999999998</v>
+      </c>
+      <c r="C26">
+        <v>0.29060000000000002</v>
+      </c>
+      <c r="D26" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26" t="s">
+        <v>28</v>
+      </c>
+      <c r="P26" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>28</v>
+      </c>
+      <c r="R26" t="s">
+        <v>28</v>
+      </c>
+      <c r="T26" t="s">
+        <v>28</v>
+      </c>
+      <c r="W26"/>
+      <c r="X26"/>
+      <c r="Y26" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB26" s="2"/>
+      <c r="AC26" s="2"/>
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>33</v>
+      </c>
+      <c r="F27" t="s">
+        <v>28</v>
+      </c>
+      <c r="P27" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>28</v>
+      </c>
+      <c r="R27" t="s">
+        <v>28</v>
+      </c>
+      <c r="T27" t="s">
+        <v>28</v>
+      </c>
+      <c r="W27"/>
+      <c r="X27"/>
+      <c r="Y27" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB27" s="2"/>
+      <c r="AC27" s="2"/>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>34</v>
+      </c>
+      <c r="F28" t="s">
+        <v>28</v>
+      </c>
+      <c r="P28" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>28</v>
+      </c>
+      <c r="R28" t="s">
+        <v>28</v>
+      </c>
+      <c r="T28" t="s">
+        <v>28</v>
+      </c>
+      <c r="W28"/>
+      <c r="X28"/>
+      <c r="Y28" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB28" s="2"/>
+      <c r="AC28" s="2"/>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>35</v>
+      </c>
+      <c r="F29" t="s">
+        <v>28</v>
+      </c>
+      <c r="P29" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>28</v>
+      </c>
+      <c r="R29" t="s">
+        <v>28</v>
+      </c>
+      <c r="T29" t="s">
+        <v>28</v>
+      </c>
+      <c r="W29"/>
+      <c r="X29"/>
+      <c r="Y29" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB29" s="2"/>
+      <c r="AC29" s="2"/>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30">
+        <v>-0.39798</v>
+      </c>
+      <c r="C30">
+        <v>0.29070000000000001</v>
+      </c>
+      <c r="D30" t="s">
+        <v>32</v>
+      </c>
+      <c r="F30" t="s">
+        <v>28</v>
+      </c>
+      <c r="S30" t="s">
+        <v>28</v>
+      </c>
+      <c r="T30" t="s">
+        <v>28</v>
+      </c>
+      <c r="W30"/>
+      <c r="X30"/>
+      <c r="Y30" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB30" s="2"/>
+      <c r="AC30" s="2"/>
+    </row>
+    <row r="31" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>33</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB31" s="3"/>
+      <c r="AC31" s="3"/>
+    </row>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F32" t="s">
+        <v>28</v>
+      </c>
+      <c r="S32" t="s">
+        <v>28</v>
+      </c>
+      <c r="T32" t="s">
+        <v>28</v>
+      </c>
+      <c r="W32"/>
+      <c r="X32"/>
+      <c r="Y32" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB32" s="2"/>
+      <c r="AC32" s="2"/>
+    </row>
+    <row r="33" spans="4:31" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>35</v>
+      </c>
+      <c r="F33" t="s">
+        <v>28</v>
+      </c>
+      <c r="S33" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T33" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="U33" s="1"/>
+      <c r="V33" s="1"/>
+      <c r="W33" s="1"/>
+      <c r="X33" s="1"/>
+      <c r="Y33" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z33" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA33" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB33" s="3"/>
+      <c r="AC33" s="3"/>
+      <c r="AD33" s="1"/>
+      <c r="AE33" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
tidying up the repo
</commit_message>
<xml_diff>
--- a/MLTracker.xlsx
+++ b/MLTracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Code\DonorsChoose\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caitlin\Desktop\cwrubootcamp\Homework\DonorsChoose\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D6A2B038-0908-484A-AF37-49DB98D87769}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C0423D2-B559-4ACB-A020-FB7F2FF0ED5B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6900" yWindow="4635" windowWidth="21900" windowHeight="7590" xr2:uid="{8BE3917C-5764-4427-A3FC-3DBEDE359AE0}"/>
+    <workbookView xWindow="-1464" yWindow="792" windowWidth="23040" windowHeight="11028" xr2:uid="{8BE3917C-5764-4427-A3FC-3DBEDE359AE0}"/>
   </bookViews>
   <sheets>
     <sheet name="No Metro" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="48">
   <si>
     <t>school_metro</t>
   </si>
@@ -164,6 +164,12 @@
   </si>
   <si>
     <t>metro_included</t>
+  </si>
+  <si>
+    <t>roc_auc_score</t>
+  </si>
+  <si>
+    <t>average_precision</t>
   </si>
 </sst>
 </file>
@@ -564,52 +570,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3B90DFA-DE1E-475C-9FD6-036A41419806}">
   <dimension ref="A1:AE33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="24" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="27.5546875" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="26" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="36.88671875" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="17" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="27.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="D1" t="s">
         <v>31</v>
@@ -696,15 +703,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>40</v>
       </c>
       <c r="B2">
-        <v>-0.39839999999999998</v>
+        <v>0.52</v>
       </c>
       <c r="C2">
-        <v>0.29399999999999998</v>
+        <v>0.71</v>
       </c>
       <c r="D2" t="s">
         <v>32</v>
@@ -773,13 +780,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B3">
-        <v>-0.7782</v>
-      </c>
-      <c r="C3">
-        <v>0.37380000000000002</v>
-      </c>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D3" t="s">
         <v>33</v>
       </c>
@@ -848,7 +849,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D4" t="s">
         <v>34</v>
       </c>
@@ -916,13 +917,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <v>-0.44740000000000002</v>
-      </c>
-      <c r="C5">
-        <v>0.30430000000000001</v>
-      </c>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
         <v>35</v>
       </c>
@@ -990,16 +985,10 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>42</v>
       </c>
-      <c r="B6">
-        <v>-0.40029999999999999</v>
-      </c>
-      <c r="C6">
-        <v>0.2944</v>
-      </c>
       <c r="D6" t="s">
         <v>32</v>
       </c>
@@ -1043,13 +1032,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B7">
-        <v>-0.78469999999999995</v>
-      </c>
-      <c r="C7">
-        <v>0.37519999999999998</v>
-      </c>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
         <v>33</v>
       </c>
@@ -1093,7 +1076,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D8" t="s">
         <v>34</v>
       </c>
@@ -1137,13 +1120,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B9">
-        <v>-0.51149999999999995</v>
-      </c>
-      <c r="C9">
-        <v>0.31780000000000003</v>
-      </c>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D9" t="s">
         <v>35</v>
       </c>
@@ -1187,16 +1164,10 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>37</v>
       </c>
-      <c r="B10">
-        <v>-0.4299</v>
-      </c>
-      <c r="C10">
-        <v>0.30059999999999998</v>
-      </c>
       <c r="D10" t="s">
         <v>32</v>
       </c>
@@ -1239,13 +1210,7 @@
       <c r="AB10"/>
       <c r="AC10"/>
     </row>
-    <row r="11" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11">
-        <v>-0.4299</v>
-      </c>
-      <c r="C11">
-        <v>0.30059999999999998</v>
-      </c>
+    <row r="11" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
         <v>33</v>
       </c>
@@ -1286,7 +1251,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
         <v>34</v>
       </c>
@@ -1329,7 +1294,7 @@
       <c r="AB12"/>
       <c r="AC12"/>
     </row>
-    <row r="13" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
         <v>35</v>
       </c>
@@ -1370,15 +1335,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>44</v>
-      </c>
-      <c r="B14">
-        <v>-0.4299</v>
-      </c>
-      <c r="C14">
-        <v>0.20066000000000001</v>
       </c>
       <c r="D14" t="s">
         <v>32</v>
@@ -1428,13 +1387,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B15">
-        <v>-0.43049999999999999</v>
-      </c>
-      <c r="C15">
-        <v>0.30070000000000002</v>
-      </c>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
         <v>33</v>
       </c>
@@ -1481,7 +1434,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
         <v>34</v>
       </c>
@@ -1489,13 +1442,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B17">
-        <v>-0.41880000000000001</v>
-      </c>
-      <c r="C17">
-        <v>0.29680000000000001</v>
-      </c>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
         <v>35</v>
       </c>
@@ -1536,16 +1483,10 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>43</v>
       </c>
-      <c r="B18">
-        <v>-0.40200000000000002</v>
-      </c>
-      <c r="C18">
-        <v>-0.29480000000000001</v>
-      </c>
       <c r="D18" t="s">
         <v>32</v>
       </c>
@@ -1565,13 +1506,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B19">
-        <v>-0.62329999999999997</v>
-      </c>
-      <c r="C19">
-        <v>0.34129999999999999</v>
-      </c>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
         <v>33</v>
       </c>
@@ -1591,7 +1526,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
         <v>34</v>
       </c>
@@ -1611,7 +1546,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
         <v>35</v>
       </c>
@@ -1631,16 +1566,10 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>38</v>
       </c>
-      <c r="B22">
-        <v>-0.4299</v>
-      </c>
-      <c r="C22">
-        <v>0.30059999999999998</v>
-      </c>
       <c r="D22" t="s">
         <v>32</v>
       </c>
@@ -1660,13 +1589,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B23">
-        <v>-0.43070000000000003</v>
-      </c>
-      <c r="C23">
-        <v>0.30080000000000001</v>
-      </c>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
         <v>33</v>
       </c>
@@ -1686,7 +1609,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
         <v>34</v>
       </c>
@@ -1706,7 +1629,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D25" t="s">
         <v>35</v>
       </c>
@@ -1726,16 +1649,10 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>39</v>
       </c>
-      <c r="B26">
-        <v>-0.40920000000000001</v>
-      </c>
-      <c r="C26">
-        <v>0.29630000000000001</v>
-      </c>
       <c r="D26" t="s">
         <v>32</v>
       </c>
@@ -1761,13 +1678,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B27">
-        <v>-0.81430000000000002</v>
-      </c>
-      <c r="C27">
-        <v>0.38150000000000001</v>
-      </c>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D27" t="s">
         <v>33</v>
       </c>
@@ -1793,7 +1704,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D28" t="s">
         <v>34</v>
       </c>
@@ -1819,13 +1730,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B29">
-        <v>-0.44140000000000001</v>
-      </c>
-      <c r="C29">
-        <v>0.30299999999999999</v>
-      </c>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D29" t="s">
         <v>35</v>
       </c>
@@ -1851,16 +1756,10 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>41</v>
       </c>
-      <c r="B30">
-        <v>-0.40260000000000001</v>
-      </c>
-      <c r="C30">
-        <v>0.2949</v>
-      </c>
       <c r="D30" t="s">
         <v>32</v>
       </c>
@@ -1883,13 +1782,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="1">
-        <v>-0.83799999999999997</v>
-      </c>
-      <c r="C31" s="1">
-        <v>0.38640000000000002</v>
-      </c>
+    <row r="31" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D31" t="s">
         <v>33</v>
       </c>
@@ -1914,13 +1807,7 @@
       <c r="AB31" s="3"/>
       <c r="AC31" s="3"/>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B32">
-        <v>-0.62460000000000004</v>
-      </c>
-      <c r="C32">
-        <v>0.34160000000000001</v>
-      </c>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D32" t="s">
         <v>34</v>
       </c>
@@ -1943,13 +1830,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B33">
-        <v>-0.43930000000000002</v>
-      </c>
-      <c r="C33">
-        <v>0.30259999999999998</v>
-      </c>
+    <row r="33" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D33" t="s">
         <v>35</v>
       </c>
@@ -1993,32 +1874,32 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.5703125" customWidth="1"/>
-    <col min="17" max="17" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.5546875" customWidth="1"/>
+    <col min="17" max="17" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="24" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="27.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="27.5546875" style="4" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="26" style="4" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="27.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -2113,7 +1994,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -2187,7 +2068,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D3" t="s">
         <v>33</v>
       </c>
@@ -2249,7 +2130,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D4" t="s">
         <v>34</v>
       </c>
@@ -2311,7 +2192,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
         <v>35</v>
       </c>
@@ -2373,7 +2254,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -2430,7 +2311,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
         <v>33</v>
       </c>
@@ -2478,7 +2359,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D8" t="s">
         <v>34</v>
       </c>
@@ -2526,7 +2407,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D9" t="s">
         <v>35</v>
       </c>
@@ -2570,7 +2451,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -2622,7 +2503,7 @@
       <c r="W10"/>
       <c r="X10"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
         <v>33</v>
       </c>
@@ -2667,7 +2548,7 @@
       <c r="AB11" s="2"/>
       <c r="AC11" s="2"/>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
         <v>34</v>
       </c>
@@ -2710,7 +2591,7 @@
       <c r="W12"/>
       <c r="X12"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
         <v>35</v>
       </c>
@@ -2755,7 +2636,7 @@
       <c r="AB13" s="2"/>
       <c r="AC13" s="2"/>
     </row>
-    <row r="14" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -2813,7 +2694,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
         <v>33</v>
       </c>
@@ -2864,7 +2745,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
         <v>34</v>
       </c>
@@ -2882,7 +2763,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
         <v>35</v>
       </c>
@@ -2933,7 +2814,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -2963,7 +2844,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
         <v>33</v>
       </c>
@@ -2984,7 +2865,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
         <v>34</v>
       </c>
@@ -3005,7 +2886,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
         <v>35</v>
       </c>
@@ -3026,7 +2907,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -3056,7 +2937,7 @@
       <c r="AB22" s="2"/>
       <c r="AC22" s="2"/>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
         <v>33</v>
       </c>
@@ -3077,7 +2958,7 @@
       <c r="AB23" s="2"/>
       <c r="AC23" s="2"/>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
         <v>34</v>
       </c>
@@ -3098,7 +2979,7 @@
       <c r="AB24" s="2"/>
       <c r="AC24" s="2"/>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D25" t="s">
         <v>35</v>
       </c>
@@ -3119,7 +3000,7 @@
       <c r="AB25" s="2"/>
       <c r="AC25" s="2"/>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -3158,7 +3039,7 @@
       <c r="AB26" s="2"/>
       <c r="AC26" s="2"/>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D27" t="s">
         <v>33</v>
       </c>
@@ -3188,7 +3069,7 @@
       <c r="AB27" s="2"/>
       <c r="AC27" s="2"/>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D28" t="s">
         <v>34</v>
       </c>
@@ -3218,7 +3099,7 @@
       <c r="AB28" s="2"/>
       <c r="AC28" s="2"/>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D29" t="s">
         <v>35</v>
       </c>
@@ -3248,7 +3129,7 @@
       <c r="AB29" s="2"/>
       <c r="AC29" s="2"/>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -3284,7 +3165,7 @@
       <c r="AB30" s="2"/>
       <c r="AC30" s="2"/>
     </row>
-    <row r="31" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D31" t="s">
         <v>33</v>
       </c>
@@ -3309,7 +3190,7 @@
       <c r="AB31" s="3"/>
       <c r="AC31" s="3"/>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D32" t="s">
         <v>34</v>
       </c>
@@ -3336,7 +3217,7 @@
       <c r="AB32" s="2"/>
       <c r="AC32" s="2"/>
     </row>
-    <row r="33" spans="4:31" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D33" t="s">
         <v>35</v>
       </c>

</xml_diff>